<commit_message>
complete code for p1
</commit_message>
<xml_diff>
--- a/Daily Reports/Coffee Shop 2.xlsx
+++ b/Daily Reports/Coffee Shop 2.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calin.grigorescu\Documents\UiPath\ExcelConsolidation\Daily Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2ed5500ba6dd79a9/Chicago projects/ExcelConsolidation_Part1/Daily Reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCAF19C-AD60-40E9-8452-6350BD5C8782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{3DCAF19C-AD60-40E9-8452-6350BD5C8782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48A88CF3-96E3-4873-BCE0-4ECF85EB54AF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="11130" windowHeight="7680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="NewSheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="NewSheet" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -409,10 +410,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA7D6E42-DF2E-4B39-AF7A-067002D394FB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>